<commit_message>
Added page object model design pattern latest
</commit_message>
<xml_diff>
--- a/TestNgpracticeexercise/testdata/caldata.xlsx
+++ b/TestNgpracticeexercise/testdata/caldata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Principle</t>
   </si>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,6 +288,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -663,7 +668,7 @@
       <c r="G2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s" s="19">
+      <c r="H2" t="s" s="24">
         <v>26</v>
       </c>
     </row>
@@ -689,7 +694,7 @@
       <c r="G3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s" s="20">
+      <c r="H3" t="s" s="25">
         <v>26</v>
       </c>
     </row>
@@ -715,7 +720,7 @@
       <c r="G4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s" s="21">
+      <c r="H4" t="s" s="26">
         <v>26</v>
       </c>
     </row>
@@ -741,7 +746,7 @@
       <c r="G5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H5" t="s" s="22">
+      <c r="H5" t="s" s="27">
         <v>26</v>
       </c>
     </row>
@@ -767,7 +772,7 @@
       <c r="G6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s" s="23">
+      <c r="H6" t="s" s="28">
         <v>27</v>
       </c>
     </row>

</xml_diff>